<commit_message>
seed for gc air
Former-commit-id: ee802ddd7976826205231d48c9eee10be129a136
</commit_message>
<xml_diff>
--- a/db/dummydata/1_hubs.xlsx
+++ b/db/dummydata/1_hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
   <si>
     <t>STATUS</t>
   </si>
@@ -142,17 +142,35 @@
     <t>Stockholm</t>
   </si>
   <si>
-    <t>ARN</t>
+    <t>STO</t>
   </si>
   <si>
     <t>190 45 Stockholm-Arlanda, Sweden</t>
+  </si>
+  <si>
+    <t>Malmo</t>
+  </si>
+  <si>
+    <t>MMX</t>
+  </si>
+  <si>
+    <t>230 32 Malmö-Sturup, Sweden</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
+    <t>1 Sky Plaza Rd, Chek Lap Kok, Hong Kong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -175,6 +193,14 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -196,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -223,6 +249,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -250,7 +282,8 @@
     <col customWidth="1" min="6" max="6" width="10.14"/>
     <col customWidth="1" min="7" max="7" width="12.14"/>
     <col customWidth="1" min="8" max="8" width="11.14"/>
-    <col customWidth="1" min="9" max="10" width="28.0"/>
+    <col customWidth="1" min="9" max="9" width="44.29"/>
+    <col customWidth="1" min="10" max="10" width="28.0"/>
     <col customWidth="1" min="11" max="27" width="8.71"/>
   </cols>
   <sheetData>
@@ -724,8 +757,61 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" ht="12.0" customHeight="1"/>
-    <row r="18" ht="12.0" customHeight="1"/>
+    <row r="17" ht="12.0" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="10">
+        <v>55.535558</v>
+      </c>
+      <c r="G17" s="10">
+        <v>13.363027</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" ht="12.0" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="10">
+        <v>22.316265</v>
+      </c>
+      <c r="G18" s="6">
+        <v>113.939724</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="19" ht="12.0" customHeight="1"/>
     <row r="20" ht="12.0" customHeight="1"/>
     <row r="21" ht="12.0" customHeight="1"/>

</xml_diff>

<commit_message>
pre merge with trucking_testing
Former-commit-id: 2b7ab474cfd9311fd10b90b610adcd721bc52feb
</commit_message>
<xml_diff>
--- a/db/dummydata/1_hubs.xlsx
+++ b/db/dummydata/1_hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>STATUS</t>
   </si>
@@ -25,9 +25,6 @@
     <t>CODE</t>
   </si>
   <si>
-    <t>OPERATOR</t>
-  </si>
-  <si>
     <t>LATITUDE</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>FULL_ADDRESS</t>
   </si>
   <si>
-    <t>TRUCKING_METHOD</t>
-  </si>
-  <si>
     <t>PHOTO</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>Port 4, Indiska Oceanen 11, 418 34 Göteborg, Sverige</t>
   </si>
   <si>
-    <t>zipcode</t>
-  </si>
-  <si>
     <t>https://assets.itsmycargo.com/assets/cityimages/Gothenburg_sm.jpg</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
     <t>Beilun Qu, Ningbo Shi, Zhejiang Sheng, China, 315800</t>
   </si>
   <si>
-    <t>city</t>
-  </si>
-  <si>
     <t>https://assets.itsmycargo.com/assets/cityimages/Ningbo_sm.jpg</t>
   </si>
   <si>
@@ -164,13 +152,43 @@
   </si>
   <si>
     <t>1 Sky Plaza Rd, Chek Lap Kok, Hong Kong</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>8, Skagerrakvej, 2100 København Ø, Denmark</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Industriestraße 102, 21107 Hamburg</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Wilhelminakade 909, 3072 AP Rotterdam, Netherlands</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -201,8 +219,18 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF999999"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +243,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor rgb="FFF5F5F5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -222,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -255,6 +289,12 @@
     <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -278,13 +318,11 @@
     <col customWidth="1" min="2" max="2" width="6.14"/>
     <col customWidth="1" min="3" max="3" width="11.43"/>
     <col customWidth="1" min="4" max="4" width="12.0"/>
-    <col customWidth="1" min="5" max="5" width="20.57"/>
-    <col customWidth="1" min="6" max="6" width="10.14"/>
-    <col customWidth="1" min="7" max="7" width="12.14"/>
-    <col customWidth="1" min="8" max="8" width="11.14"/>
-    <col customWidth="1" min="9" max="9" width="44.29"/>
-    <col customWidth="1" min="10" max="10" width="28.0"/>
-    <col customWidth="1" min="11" max="27" width="8.71"/>
+    <col customWidth="1" min="5" max="5" width="10.14"/>
+    <col customWidth="1" min="6" max="6" width="12.14"/>
+    <col customWidth="1" min="7" max="7" width="11.14"/>
+    <col customWidth="1" min="8" max="8" width="63.71"/>
+    <col customWidth="1" min="9" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
@@ -312,15 +350,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -335,488 +369,548 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="5">
+        <v>57.694253</v>
+      </c>
+      <c r="F2" s="6">
+        <v>11.854048</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5">
-        <v>57.694253</v>
-      </c>
-      <c r="G2" s="6">
-        <v>11.854048</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" ht="12.0" customHeight="1">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5">
+        <v>29.929641</v>
+      </c>
+      <c r="F3" s="6">
+        <v>121.84597</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="5">
-        <v>29.929641</v>
-      </c>
-      <c r="G3" s="6">
-        <v>121.84597</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="E4" s="7">
+        <v>30.626539</v>
       </c>
       <c r="F4" s="7">
-        <v>30.626539</v>
-      </c>
-      <c r="G4" s="7">
         <v>122.064958</v>
       </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="5" t="s">
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5">
         <v>38.926974</v>
       </c>
-      <c r="G5" s="6">
+      <c r="F5" s="6">
         <v>121.655672</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="5">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5">
         <v>36.083811</v>
       </c>
-      <c r="G6" s="6">
+      <c r="F6" s="6">
         <v>120.323534</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5">
         <v>22.544083</v>
       </c>
-      <c r="G7" s="6">
+      <c r="F7" s="6">
         <v>113.899893</v>
       </c>
+      <c r="G7" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="H7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="5">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5">
         <v>38.993914</v>
       </c>
-      <c r="G8" s="6">
+      <c r="F8" s="6">
         <v>117.721024</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="E9" s="7">
         <v>57.668079</v>
       </c>
-      <c r="G9" s="5">
+      <c r="F9" s="5">
         <v>12.291456</v>
       </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5">
+        <v>29.826602</v>
+      </c>
+      <c r="F10" s="6">
+        <v>121.462084</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="5">
-        <v>29.826602</v>
-      </c>
-      <c r="G10" s="6">
-        <v>121.462084</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="5">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5">
         <v>31.141906</v>
       </c>
-      <c r="G11" s="6">
+      <c r="F11" s="6">
         <v>121.813579</v>
       </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="5" t="s">
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" ht="12.0" customHeight="1">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5">
+        <v>38.96542</v>
+      </c>
+      <c r="F12" s="6">
+        <v>121.539683</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="5">
-        <v>38.96542</v>
-      </c>
-      <c r="G12" s="6">
-        <v>121.539683</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="5">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5">
         <v>36.266199</v>
       </c>
-      <c r="G13" s="6">
+      <c r="F13" s="6">
         <v>120.383413</v>
       </c>
+      <c r="G13" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="H13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="5">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5">
         <v>22.634996</v>
       </c>
-      <c r="G14" s="6">
+      <c r="F14" s="6">
         <v>113.812407</v>
       </c>
+      <c r="G14" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="H14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="5">
+        <v>28</v>
+      </c>
+      <c r="E15" s="5">
         <v>39.130656</v>
       </c>
-      <c r="G15" s="6">
+      <c r="F15" s="6">
         <v>117.35817</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="E16" s="9">
+        <v>59.650856</v>
       </c>
       <c r="F16" s="9">
-        <v>59.650856</v>
-      </c>
-      <c r="G16" s="9">
         <v>17.931097</v>
       </c>
+      <c r="G16" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="E17" s="10">
+        <v>55.535558</v>
       </c>
       <c r="F17" s="10">
-        <v>55.535558</v>
-      </c>
-      <c r="G17" s="10">
         <v>13.363027</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>16</v>
+      <c r="G17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="10">
+        <v>22.316265</v>
+      </c>
+      <c r="F18" s="6">
+        <v>113.939724</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" ht="12.0" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="12">
+        <v>55.694864</v>
+      </c>
+      <c r="F19" s="6">
+        <v>12.614036</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="10">
+    </row>
+    <row r="20" ht="12.0" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="12">
+        <v>53.536975</v>
+      </c>
+      <c r="F20" s="6">
+        <v>9.918213</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" ht="12.0" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="10">
         <v>22.316265</v>
       </c>
-      <c r="G18" s="6">
+      <c r="F21" s="6">
         <v>113.939724</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" ht="12.0" customHeight="1"/>
-    <row r="20" ht="12.0" customHeight="1"/>
-    <row r="21" ht="12.0" customHeight="1"/>
-    <row r="22" ht="12.0" customHeight="1"/>
-    <row r="23" ht="12.0" customHeight="1"/>
+      <c r="G21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" ht="12.0" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1.26666667</v>
+      </c>
+      <c r="F22" s="5">
+        <v>103.83333333</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" ht="12.0" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="12">
+        <v>51.904809</v>
+      </c>
+      <c r="F23" s="6">
+        <v>4.484179</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="24" ht="12.0" customHeight="1"/>
     <row r="25" ht="12.0" customHeight="1"/>
     <row r="26" ht="12.0" customHeight="1"/>
@@ -1789,12 +1883,12 @@
     <row r="993" ht="12.0" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="K2"/>
-    <hyperlink r:id="rId2" ref="K3"/>
-    <hyperlink r:id="rId3" ref="K4"/>
-    <hyperlink r:id="rId4" ref="K9"/>
-    <hyperlink r:id="rId5" ref="K10"/>
-    <hyperlink r:id="rId6" ref="K11"/>
+    <hyperlink r:id="rId1" ref="I2"/>
+    <hyperlink r:id="rId2" ref="I3"/>
+    <hyperlink r:id="rId3" ref="I4"/>
+    <hyperlink r:id="rId4" ref="I9"/>
+    <hyperlink r:id="rId5" ref="I10"/>
+    <hyperlink r:id="rId6" ref="I11"/>
   </hyperlinks>
   <drawing r:id="rId7"/>
 </worksheet>

</xml_diff>